<commit_message>
improved descriptions and separated volunteer work that are not really related but are cool to keep
</commit_message>
<xml_diff>
--- a/shira_salingre_cv_data.xlsx
+++ b/shira_salingre_cv_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shirasalin\Documents\Work\my_cv\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{17C4CE7F-6EA3-4B61-92D6-C3CA50E2C741}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C93042D7-FFE0-4B8C-AD2C-AD46A59EEBEE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{F213A91E-98B5-B244-B12A-A608C8962BCD}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="5" xr2:uid="{F213A91E-98B5-B244-B12A-A608C8962BCD}"/>
   </bookViews>
   <sheets>
     <sheet name="education" sheetId="10" r:id="rId1"/>
@@ -18,7 +18,7 @@
     <sheet name="skills" sheetId="8" r:id="rId3"/>
     <sheet name="languages" sheetId="12" r:id="rId4"/>
     <sheet name="research" sheetId="5" r:id="rId5"/>
-    <sheet name="leadership" sheetId="7" r:id="rId6"/>
+    <sheet name="volunteer" sheetId="7" r:id="rId6"/>
     <sheet name="not_included" sheetId="11" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029"/>
@@ -42,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="79">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="83">
   <si>
     <t>institution</t>
   </si>
@@ -185,9 +185,6 @@
     <t>The National Sea Turtle Rescue Center, NPA</t>
   </si>
   <si>
-    <t>Sea turtle care taker volunteer</t>
-  </si>
-  <si>
     <t>Invasive sea star removal volunteer</t>
   </si>
   <si>
@@ -206,9 +203,6 @@
     <t>Eye of the Whale</t>
   </si>
   <si>
-    <t>Cleaned and fed turtles and helped when needed in medical operations. It was great fun!</t>
-  </si>
-  <si>
     <t>While living and working in Melbourne I took part in physically removing invasive northern pacific seastar from Port Phillip bay.</t>
   </si>
   <si>
@@ -230,9 +224,6 @@
     <t>Today</t>
   </si>
   <si>
-    <t>Worked on various ecological project as part of the Ruppin Estuarine Coastal Observatory (RECO), where I collected samples, extracted biological and chemical indicators from them and assisted with other projects on marine ascidians.</t>
-  </si>
-  <si>
     <t>Learned and practiced most of my data science skills, mainly using R, Rstudio (now ‘posit’) and GitHub.</t>
   </si>
   <si>
@@ -260,12 +251,6 @@
     <t>Data cleaning and analysis for in various ecological research projects.</t>
   </si>
   <si>
-    <t>Coordinated and managed a team of volunteers of a regional sea turtle hatchery, throughout the hatching season. As part of my work I also had to update and consult the hatching database for our operations.</t>
-  </si>
-  <si>
-    <t>Analysed and processed large data sets R, SQL queries, QGIS, ArcGIS, Excel and Google Sheets.</t>
-  </si>
-  <si>
     <t>Managed, processed, analysed and visualised ecological data to create reports for professional resrearchers and the general public.</t>
   </si>
   <si>
@@ -279,6 +264,33 @@
   </si>
   <si>
     <t>CSS</t>
+  </si>
+  <si>
+    <t>Worked with large data sets using R, QGIS, ArcGIS, Microsoft Excel and Google Sheets.</t>
+  </si>
+  <si>
+    <t>Collected, organised and analysed these data using Google Sheets, Microsoft Excel and R.</t>
+  </si>
+  <si>
+    <t>Used SQL queries for pulling data from a database in fulcrum.</t>
+  </si>
+  <si>
+    <t>In 2017 I done this job again</t>
+  </si>
+  <si>
+    <t>Using R for data cleaning, ecological analysis and visualisation. Wiritng reports that include graphics I created and communicating my work to my clients using presentations and Rmarkdown.</t>
+  </si>
+  <si>
+    <t>Collected samples, extracted biological and chemical indicators from them and assisted with other projects on marine ascidians.</t>
+  </si>
+  <si>
+    <t>Worked on various ecological project as part of the Ruppin Estuarine Coastal Observatory (RECO).</t>
+  </si>
+  <si>
+    <t>Coordinated and managed a team of volunteers of a regional sea turtle hatchery, throughout the hatching season.</t>
+  </si>
+  <si>
+    <t>As part of my work I also had to update and consult the hatching database for our operations.</t>
   </si>
 </sst>
 </file>
@@ -692,7 +704,7 @@
         <v>18</v>
       </c>
       <c r="E2" t="s">
-        <v>63</v>
+        <v>60</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
@@ -709,7 +721,7 @@
         <v>18</v>
       </c>
       <c r="E3" t="s">
-        <v>70</v>
+        <v>67</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
@@ -726,7 +738,7 @@
         <v>18</v>
       </c>
       <c r="E4" t="s">
-        <v>64</v>
+        <v>61</v>
       </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.25">
@@ -754,10 +766,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C980247-8D3C-E442-A656-D4E45E07EA31}">
-  <dimension ref="A1:G17"/>
+  <dimension ref="A1:G19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+      <selection activeCell="A20" sqref="A20:XFD21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -799,13 +811,13 @@
         <v>2015</v>
       </c>
       <c r="E2" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="F2" t="s">
         <v>26</v>
       </c>
       <c r="G2" t="s">
-        <v>71</v>
+        <v>68</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
@@ -819,36 +831,33 @@
         <v>2015</v>
       </c>
       <c r="E3" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="F3" t="s">
         <v>26</v>
       </c>
       <c r="G3" t="s">
-        <v>27</v>
+        <v>78</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="B4" t="s">
-        <v>29</v>
-      </c>
-      <c r="C4" t="s">
-        <v>18</v>
+        <v>25</v>
       </c>
       <c r="D4">
-        <v>2020</v>
-      </c>
-      <c r="E4">
-        <v>2022</v>
+        <v>2015</v>
+      </c>
+      <c r="E4" t="s">
+        <v>59</v>
       </c>
       <c r="F4" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="G4" t="s">
-        <v>74</v>
+        <v>27</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
@@ -871,282 +880,280 @@
         <v>30</v>
       </c>
       <c r="G5" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>31</v>
+        <v>28</v>
       </c>
       <c r="B6" t="s">
-        <v>21</v>
+        <v>29</v>
       </c>
       <c r="C6" t="s">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="D6">
-        <v>2019</v>
+        <v>2020</v>
       </c>
       <c r="E6">
         <v>2022</v>
       </c>
-      <c r="F6" t="str">
-        <f>_xlfn.CONCAT(D6,"--",E6)</f>
-        <v>2019--2022</v>
+      <c r="F6" t="s">
+        <v>30</v>
       </c>
       <c r="G6" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="B7" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="C7" t="s">
-        <v>38</v>
+        <v>18</v>
       </c>
       <c r="D7">
-        <v>2007</v>
+        <v>2020</v>
       </c>
       <c r="E7">
-        <v>2019</v>
-      </c>
-      <c r="F7" t="str">
-        <f t="shared" ref="F7:F12" si="0">_xlfn.CONCAT(D7,"--",E7)</f>
-        <v>2007--2019</v>
+        <v>2022</v>
+      </c>
+      <c r="F7" t="s">
+        <v>30</v>
       </c>
       <c r="G7" t="s">
-        <v>34</v>
+        <v>76</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B8" t="s">
-        <v>33</v>
+        <v>21</v>
       </c>
       <c r="C8" t="s">
-        <v>38</v>
+        <v>22</v>
       </c>
       <c r="D8">
-        <v>2007</v>
+        <v>2019</v>
       </c>
       <c r="E8">
-        <v>2019</v>
+        <v>2022</v>
       </c>
       <c r="F8" t="str">
-        <f t="shared" si="0"/>
-        <v>2007--2019</v>
+        <f>_xlfn.CONCAT(D8,"--",E8)</f>
+        <v>2019--2022</v>
       </c>
       <c r="G8" t="s">
-        <v>35</v>
+        <v>70</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="B9" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="C9" t="s">
         <v>38</v>
       </c>
       <c r="D9">
-        <v>2014</v>
+        <v>2007</v>
       </c>
       <c r="E9">
         <v>2019</v>
       </c>
       <c r="F9" t="str">
-        <f t="shared" si="0"/>
-        <v>2014--2019</v>
+        <f>_xlfn.CONCAT(D9,"--",E9)</f>
+        <v>2007--2019</v>
       </c>
       <c r="G9" t="s">
-        <v>39</v>
+        <v>34</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="B10" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="C10" t="s">
         <v>38</v>
       </c>
       <c r="D10">
-        <v>2014</v>
+        <v>2007</v>
       </c>
       <c r="E10">
         <v>2019</v>
       </c>
       <c r="F10" t="str">
-        <f t="shared" si="0"/>
-        <v>2014--2019</v>
+        <f>_xlfn.CONCAT(D10,"--",E10)</f>
+        <v>2007--2019</v>
       </c>
       <c r="G10" t="s">
-        <v>76</v>
+        <v>35</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="B11" t="s">
-        <v>41</v>
+        <v>37</v>
       </c>
       <c r="C11" t="s">
         <v>38</v>
       </c>
       <c r="D11">
-        <v>2016</v>
+        <v>2014</v>
       </c>
       <c r="E11">
-        <v>2018</v>
+        <v>2019</v>
       </c>
       <c r="F11" t="str">
-        <f t="shared" si="0"/>
-        <v>2016--2018</v>
+        <f>_xlfn.CONCAT(D11,"--",E11)</f>
+        <v>2014--2019</v>
       </c>
       <c r="G11" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>43</v>
+        <v>36</v>
       </c>
       <c r="B12" t="s">
-        <v>44</v>
+        <v>37</v>
       </c>
       <c r="C12" t="s">
-        <v>22</v>
+        <v>38</v>
       </c>
       <c r="D12">
-        <v>2016</v>
+        <v>2014</v>
       </c>
       <c r="E12">
-        <v>2018</v>
+        <v>2019</v>
       </c>
       <c r="F12" t="str">
-        <f t="shared" si="0"/>
-        <v>2016--2018</v>
+        <f>_xlfn.CONCAT(D12,"--",E12)</f>
+        <v>2014--2019</v>
       </c>
       <c r="G12" t="s">
-        <v>62</v>
+        <v>75</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>45</v>
+        <v>36</v>
       </c>
       <c r="B13" t="s">
-        <v>46</v>
+        <v>37</v>
       </c>
       <c r="C13" t="s">
-        <v>22</v>
+        <v>38</v>
       </c>
       <c r="D13">
-        <v>2011</v>
+        <v>2014</v>
       </c>
       <c r="E13">
-        <v>2011</v>
+        <v>2019</v>
       </c>
       <c r="F13" t="str">
         <f>_xlfn.CONCAT(D13,"--",E13)</f>
-        <v>2011--2011</v>
+        <v>2014--2019</v>
       </c>
       <c r="G13" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>45</v>
+        <v>40</v>
       </c>
       <c r="B14" t="s">
-        <v>46</v>
+        <v>41</v>
       </c>
       <c r="C14" t="s">
-        <v>22</v>
+        <v>38</v>
       </c>
       <c r="D14">
-        <v>2017</v>
+        <v>2016</v>
       </c>
       <c r="E14">
-        <v>2017</v>
+        <v>2018</v>
       </c>
       <c r="F14" t="str">
         <f>_xlfn.CONCAT(D14,"--",E14)</f>
-        <v>2017--2017</v>
+        <v>2016--2018</v>
       </c>
       <c r="G14" t="s">
-        <v>72</v>
+        <v>42</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>47</v>
+        <v>43</v>
       </c>
       <c r="B15" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C15" t="s">
         <v>22</v>
       </c>
       <c r="D15">
-        <v>2009</v>
+        <v>2016</v>
       </c>
       <c r="E15">
-        <v>2016</v>
+        <v>2018</v>
       </c>
       <c r="F15" t="str">
         <f>_xlfn.CONCAT(D15,"--",E15)</f>
-        <v>2009--2016</v>
+        <v>2016--2018</v>
       </c>
       <c r="G15" t="s">
-        <v>54</v>
+        <v>80</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="B16" t="s">
-        <v>52</v>
+        <v>44</v>
       </c>
       <c r="C16" t="s">
-        <v>50</v>
+        <v>22</v>
       </c>
       <c r="D16">
-        <v>2013</v>
+        <v>2016</v>
       </c>
       <c r="E16">
-        <v>2013</v>
+        <v>2018</v>
       </c>
       <c r="F16" t="str">
         <f>_xlfn.CONCAT(D16,"--",E16)</f>
-        <v>2013--2013</v>
+        <v>2016--2018</v>
       </c>
       <c r="G16" t="s">
-        <v>55</v>
+        <v>79</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>49</v>
+        <v>45</v>
       </c>
       <c r="B17" t="s">
-        <v>53</v>
+        <v>46</v>
       </c>
       <c r="C17" t="s">
-        <v>51</v>
+        <v>22</v>
       </c>
       <c r="D17">
         <v>2011</v>
@@ -1159,7 +1166,55 @@
         <v>2011--2011</v>
       </c>
       <c r="G17" t="s">
-        <v>56</v>
+        <v>81</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>45</v>
+      </c>
+      <c r="B18" t="s">
+        <v>46</v>
+      </c>
+      <c r="C18" t="s">
+        <v>22</v>
+      </c>
+      <c r="D18">
+        <v>2011</v>
+      </c>
+      <c r="E18">
+        <v>2011</v>
+      </c>
+      <c r="F18" t="str">
+        <f>_xlfn.CONCAT(D18,"--",E18)</f>
+        <v>2011--2011</v>
+      </c>
+      <c r="G18" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>45</v>
+      </c>
+      <c r="B19" t="s">
+        <v>46</v>
+      </c>
+      <c r="C19" t="s">
+        <v>22</v>
+      </c>
+      <c r="D19">
+        <v>2011</v>
+      </c>
+      <c r="E19">
+        <v>2011</v>
+      </c>
+      <c r="F19" t="str">
+        <f>_xlfn.CONCAT(D19,"--",E19)</f>
+        <v>2011--2011</v>
+      </c>
+      <c r="G19" t="s">
+        <v>77</v>
       </c>
     </row>
   </sheetData>
@@ -1172,7 +1227,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7F75B33B-21C6-D44F-A780-FE0F5972B759}">
   <dimension ref="A1:B10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
@@ -1196,7 +1251,7 @@
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B3">
         <v>5</v>
@@ -1204,7 +1259,7 @@
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="B4">
         <v>4</v>
@@ -1212,7 +1267,7 @@
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B5">
         <v>4</v>
@@ -1220,7 +1275,7 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="B6">
         <v>3.5</v>
@@ -1244,7 +1299,7 @@
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
       <c r="B9">
         <v>4</v>
@@ -1252,7 +1307,7 @@
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="B10">
         <v>2</v>
@@ -1283,26 +1338,26 @@
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>62</v>
+      </c>
+      <c r="B2" t="s">
         <v>65</v>
-      </c>
-      <c r="B2" t="s">
-        <v>68</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>66</v>
+        <v>63</v>
       </c>
       <c r="B3" t="s">
-        <v>68</v>
+        <v>65</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>67</v>
+        <v>64</v>
       </c>
       <c r="B4" t="s">
-        <v>69</v>
+        <v>66</v>
       </c>
     </row>
   </sheetData>
@@ -1377,7 +1432,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B0C1DA58-DF2A-1948-9210-AF2DD0CDBCFC}">
   <dimension ref="A1:G3"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G2" sqref="G2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
@@ -1404,21 +1461,53 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A2" s="1"/>
-      <c r="B2" s="1"/>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
-      <c r="G2" s="1"/>
-    </row>
-    <row r="3" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A3" s="1"/>
-      <c r="B3" s="1"/>
-      <c r="C3" s="1"/>
-      <c r="D3" s="1"/>
-      <c r="E3" s="1"/>
-      <c r="G3" s="1"/>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>47</v>
+      </c>
+      <c r="B2" t="s">
+        <v>51</v>
+      </c>
+      <c r="C2" t="s">
+        <v>49</v>
+      </c>
+      <c r="D2">
+        <v>2013</v>
+      </c>
+      <c r="E2">
+        <v>2013</v>
+      </c>
+      <c r="F2" t="str">
+        <f>_xlfn.CONCAT(D2,"--",E2)</f>
+        <v>2013--2013</v>
+      </c>
+      <c r="G2" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>48</v>
+      </c>
+      <c r="B3" t="s">
+        <v>52</v>
+      </c>
+      <c r="C3" t="s">
+        <v>50</v>
+      </c>
+      <c r="D3">
+        <v>2011</v>
+      </c>
+      <c r="E3">
+        <v>2011</v>
+      </c>
+      <c r="F3" t="str">
+        <f>_xlfn.CONCAT(D3,"--",E3)</f>
+        <v>2011--2011</v>
+      </c>
+      <c r="G3" t="s">
+        <v>54</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
added more information and improved skills section
</commit_message>
<xml_diff>
--- a/shira_salingre_cv_data.xlsx
+++ b/shira_salingre_cv_data.xlsx
@@ -8,18 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shirasalin\Documents\Work\my_cv\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C93042D7-FFE0-4B8C-AD2C-AD46A59EEBEE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AC413E78-3FFE-4460-9DE2-8B4A8D51388D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="5" xr2:uid="{F213A91E-98B5-B244-B12A-A608C8962BCD}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{F213A91E-98B5-B244-B12A-A608C8962BCD}"/>
   </bookViews>
   <sheets>
     <sheet name="education" sheetId="10" r:id="rId1"/>
     <sheet name="industry" sheetId="6" r:id="rId2"/>
     <sheet name="skills" sheetId="8" r:id="rId3"/>
-    <sheet name="languages" sheetId="12" r:id="rId4"/>
-    <sheet name="research" sheetId="5" r:id="rId5"/>
-    <sheet name="volunteer" sheetId="7" r:id="rId6"/>
-    <sheet name="not_included" sheetId="11" r:id="rId7"/>
+    <sheet name="research" sheetId="5" r:id="rId4"/>
+    <sheet name="volunteer" sheetId="7" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -42,17 +40,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="158" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="82">
   <si>
     <t>institution</t>
   </si>
   <si>
-    <t>skill</t>
-  </si>
-  <si>
-    <t>level</t>
-  </si>
-  <si>
     <t>R</t>
   </si>
   <si>
@@ -86,9 +78,6 @@
     <t>dates</t>
   </si>
   <si>
-    <t>language</t>
-  </si>
-  <si>
     <t>MSc, Ecology</t>
   </si>
   <si>
@@ -116,45 +105,21 @@
     <t>Learned basics of research methods, including data analysis using GIS software and Microsoft Excel. My studies included a research project on the effects of fish farms in open seas.</t>
   </si>
   <si>
-    <t>Marine ecology specialist</t>
-  </si>
-  <si>
     <t>Freelance</t>
   </si>
   <si>
     <t>2015--Present</t>
   </si>
   <si>
-    <t>Professional adviser and project coordinator for a multitude of projects, mainly focusing on creating educational and professional materials on marine ecology and conservation.</t>
-  </si>
-  <si>
-    <t>Data projects ecologist</t>
-  </si>
-  <si>
     <t>HaMaarag - Israel’s Nature Assessment Program</t>
   </si>
   <si>
     <t>2020--2022</t>
   </si>
   <si>
-    <t>Teaching assistant in BSc course</t>
-  </si>
-  <si>
-    <t>Nature conservation tour guide</t>
-  </si>
-  <si>
     <t>Nature and Parks Authority</t>
   </si>
   <si>
-    <t>Guided nature-conservation oriented tours, in field trips and in classes or lectures.</t>
-  </si>
-  <si>
-    <t>Lead long-term ecological and environmental educational projects.</t>
-  </si>
-  <si>
-    <t>Elasmobranch researcher</t>
-  </si>
-  <si>
     <t>Sharks in Israel</t>
   </si>
   <si>
@@ -164,9 +129,6 @@
     <t>Established and managed a shark and rays citizen science observation database.</t>
   </si>
   <si>
-    <t>Recreational fishing surveyor</t>
-  </si>
-  <si>
     <t>Nature and Parks Authority &amp; Tel Aviv University</t>
   </si>
   <si>
@@ -179,9 +141,6 @@
     <t>Gitai Yahel's lab, Ruppin Academic Center</t>
   </si>
   <si>
-    <t>Sea turtle hatching season volunteer coordinator</t>
-  </si>
-  <si>
     <t>The National Sea Turtle Rescue Center, NPA</t>
   </si>
   <si>
@@ -224,33 +183,15 @@
     <t>Today</t>
   </si>
   <si>
-    <t>Learned and practiced most of my data science skills, mainly using R, Rstudio (now ‘posit’) and GitHub.</t>
-  </si>
-  <si>
-    <t>Research topic: “Dynamics of fish networks along environmental gradients in the Mediterranean Sea".</t>
-  </si>
-  <si>
     <t>Hebrew</t>
   </si>
   <si>
     <t>English</t>
   </si>
   <si>
-    <t>Spanish (Castellano)</t>
-  </si>
-  <si>
-    <t>C2</t>
-  </si>
-  <si>
-    <t>B1</t>
-  </si>
-  <si>
     <t>Started a Github account for our lab, initiated a Google website platform for lab's fish identification guide, gathered and cleaned our Mediterranean database and lead lab hackathons.</t>
   </si>
   <si>
-    <t>Data cleaning and analysis for in various ecological research projects.</t>
-  </si>
-  <si>
     <t>Managed, processed, analysed and visualised ecological data to create reports for professional resrearchers and the general public.</t>
   </si>
   <si>
@@ -272,25 +213,79 @@
     <t>Collected, organised and analysed these data using Google Sheets, Microsoft Excel and R.</t>
   </si>
   <si>
-    <t>Used SQL queries for pulling data from a database in fulcrum.</t>
-  </si>
-  <si>
     <t>In 2017 I done this job again</t>
   </si>
   <si>
-    <t>Using R for data cleaning, ecological analysis and visualisation. Wiritng reports that include graphics I created and communicating my work to my clients using presentations and Rmarkdown.</t>
-  </si>
-  <si>
     <t>Collected samples, extracted biological and chemical indicators from them and assisted with other projects on marine ascidians.</t>
   </si>
   <si>
-    <t>Worked on various ecological project as part of the Ruppin Estuarine Coastal Observatory (RECO).</t>
-  </si>
-  <si>
-    <t>Coordinated and managed a team of volunteers of a regional sea turtle hatchery, throughout the hatching season.</t>
-  </si>
-  <si>
-    <t>As part of my work I also had to update and consult the hatching database for our operations.</t>
+    <t>Built my data science skills, mainly using R, Rstudio (now ‘posit’) and GitHub.</t>
+  </si>
+  <si>
+    <t>Marine ecologist and analyst</t>
+  </si>
+  <si>
+    <t>Data specialist</t>
+  </si>
+  <si>
+    <t>Teaching assistant</t>
+  </si>
+  <si>
+    <t>Nature guide</t>
+  </si>
+  <si>
+    <t>Data collector</t>
+  </si>
+  <si>
+    <t>Volunteer coordinator</t>
+  </si>
+  <si>
+    <t>Cleaned, analysed and reported data for various ecological research projects</t>
+  </si>
+  <si>
+    <t>Database administrator</t>
+  </si>
+  <si>
+    <t>Professional adviser and project coordinator for a multitude of projects, mainly creating educational and professional materials on marine ecology and conservation.</t>
+  </si>
+  <si>
+    <t>Used SQL queries to pull data from a database in fulcrum.</t>
+  </si>
+  <si>
+    <t>Guided nature-conservation oriented tours, in field trips and in classes or lectures and lead long-term ecological and environmental educational projects.</t>
+  </si>
+  <si>
+    <t>Coordinated and managed a team of volunteers of a regional sea turtle hatchery, throughout the hatching season. Update and consulted the hatchery database for daily operations.</t>
+  </si>
+  <si>
+    <t>Type</t>
+  </si>
+  <si>
+    <t>Skill</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Tech Stack</t>
+  </si>
+  <si>
+    <t>C2 - Native</t>
+  </si>
+  <si>
+    <t>C2 - Fluent</t>
+  </si>
+  <si>
+    <t>B1 - Intermediate</t>
+  </si>
+  <si>
+    <t>Score</t>
+  </si>
+  <si>
+    <t>Language</t>
+  </si>
+  <si>
+    <t>Spanish</t>
   </si>
 </sst>
 </file>
@@ -658,11 +653,9 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9C4AE3D1-7C9F-C24D-A42B-F2C4925E72DD}">
-  <dimension ref="A1:E5"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
+    <sheetView zoomScaleNormal="100" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -675,87 +668,70 @@
   <sheetData>
     <row r="1" spans="1:5" s="2" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B1" s="2" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="E1" s="2" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B2" t="s">
+        <v>13</v>
+      </c>
+      <c r="C2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2" t="s">
         <v>15</v>
       </c>
-      <c r="B2" t="s">
-        <v>16</v>
-      </c>
-      <c r="C2" t="s">
-        <v>17</v>
-      </c>
-      <c r="D2" t="s">
-        <v>18</v>
-      </c>
       <c r="E2" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>12</v>
+      </c>
+      <c r="B3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D3" t="s">
         <v>15</v>
       </c>
-      <c r="B3" t="s">
-        <v>16</v>
-      </c>
-      <c r="C3" t="s">
-        <v>17</v>
-      </c>
-      <c r="D3" t="s">
-        <v>18</v>
-      </c>
       <c r="E3" t="s">
-        <v>67</v>
+        <v>49</v>
       </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B4" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="C4" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="D4" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="E4" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>19</v>
-      </c>
-      <c r="B5" t="s">
         <v>20</v>
-      </c>
-      <c r="C5" t="s">
-        <v>21</v>
-      </c>
-      <c r="D5" t="s">
-        <v>22</v>
-      </c>
-      <c r="E5" t="s">
-        <v>23</v>
       </c>
     </row>
   </sheetData>
@@ -766,10 +742,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C980247-8D3C-E442-A656-D4E45E07EA31}">
-  <dimension ref="A1:G19"/>
+  <dimension ref="A1:G15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A20" sqref="A20:XFD21"/>
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -779,96 +755,99 @@
   <sheetData>
     <row r="1" spans="1:7" s="2" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="E1" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>13</v>
-      </c>
       <c r="G1" s="2" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>24</v>
+        <v>60</v>
       </c>
       <c r="B2" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="D2">
         <v>2015</v>
       </c>
       <c r="E2" t="s">
-        <v>59</v>
+        <v>46</v>
       </c>
       <c r="F2" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="G2" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>24</v>
+        <v>60</v>
       </c>
       <c r="B3" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="D3">
         <v>2015</v>
       </c>
       <c r="E3" t="s">
-        <v>59</v>
+        <v>46</v>
       </c>
       <c r="F3" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="G3" t="s">
-        <v>78</v>
+        <v>68</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>61</v>
+      </c>
+      <c r="B4" t="s">
+        <v>23</v>
+      </c>
+      <c r="C4" t="s">
+        <v>15</v>
+      </c>
+      <c r="D4">
+        <v>2020</v>
+      </c>
+      <c r="E4">
+        <v>2022</v>
+      </c>
+      <c r="F4" t="s">
         <v>24</v>
       </c>
-      <c r="B4" t="s">
-        <v>25</v>
-      </c>
-      <c r="D4">
-        <v>2015</v>
-      </c>
-      <c r="E4" t="s">
-        <v>59</v>
-      </c>
-      <c r="F4" t="s">
-        <v>26</v>
-      </c>
       <c r="G4" t="s">
-        <v>27</v>
+        <v>50</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>28</v>
+        <v>61</v>
       </c>
       <c r="B5" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="C5" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="D5">
         <v>2020</v>
@@ -877,21 +856,21 @@
         <v>2022</v>
       </c>
       <c r="F5" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="G5" t="s">
-        <v>69</v>
+        <v>55</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>28</v>
+        <v>61</v>
       </c>
       <c r="B6" t="s">
-        <v>29</v>
+        <v>23</v>
       </c>
       <c r="C6" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="D6">
         <v>2020</v>
@@ -900,54 +879,55 @@
         <v>2022</v>
       </c>
       <c r="F6" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="G6" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>28</v>
+        <v>62</v>
       </c>
       <c r="B7" t="s">
-        <v>29</v>
+        <v>18</v>
       </c>
       <c r="C7" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="D7">
-        <v>2020</v>
+        <v>2019</v>
       </c>
       <c r="E7">
         <v>2022</v>
       </c>
-      <c r="F7" t="s">
-        <v>30</v>
+      <c r="F7" t="str">
+        <f t="shared" ref="F7:F15" si="0">_xlfn.CONCAT(D7,"--",E7)</f>
+        <v>2019--2022</v>
       </c>
       <c r="G7" t="s">
-        <v>76</v>
+        <v>51</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>31</v>
+        <v>63</v>
       </c>
       <c r="B8" t="s">
-        <v>21</v>
+        <v>25</v>
       </c>
       <c r="C8" t="s">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="D8">
+        <v>2007</v>
+      </c>
+      <c r="E8">
         <v>2019</v>
       </c>
-      <c r="E8">
-        <v>2022</v>
-      </c>
       <c r="F8" t="str">
-        <f>_xlfn.CONCAT(D8,"--",E8)</f>
-        <v>2019--2022</v>
+        <f t="shared" si="0"/>
+        <v>2007--2019</v>
       </c>
       <c r="G8" t="s">
         <v>70</v>
@@ -955,61 +935,61 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>32</v>
+        <v>67</v>
       </c>
       <c r="B9" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="C9" t="s">
-        <v>38</v>
+        <v>27</v>
       </c>
       <c r="D9">
-        <v>2007</v>
+        <v>2014</v>
       </c>
       <c r="E9">
         <v>2019</v>
       </c>
       <c r="F9" t="str">
-        <f>_xlfn.CONCAT(D9,"--",E9)</f>
-        <v>2007--2019</v>
+        <f t="shared" si="0"/>
+        <v>2014--2019</v>
       </c>
       <c r="G9" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>32</v>
+        <v>67</v>
       </c>
       <c r="B10" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
       <c r="C10" t="s">
-        <v>38</v>
+        <v>27</v>
       </c>
       <c r="D10">
-        <v>2007</v>
+        <v>2014</v>
       </c>
       <c r="E10">
         <v>2019</v>
       </c>
       <c r="F10" t="str">
-        <f>_xlfn.CONCAT(D10,"--",E10)</f>
-        <v>2007--2019</v>
+        <f t="shared" si="0"/>
+        <v>2014--2019</v>
       </c>
       <c r="G10" t="s">
-        <v>35</v>
+        <v>56</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>36</v>
+        <v>67</v>
       </c>
       <c r="B11" t="s">
-        <v>37</v>
+        <v>26</v>
       </c>
       <c r="C11" t="s">
-        <v>38</v>
+        <v>27</v>
       </c>
       <c r="D11">
         <v>2014</v>
@@ -1018,203 +998,107 @@
         <v>2019</v>
       </c>
       <c r="F11" t="str">
-        <f>_xlfn.CONCAT(D11,"--",E11)</f>
+        <f t="shared" si="0"/>
         <v>2014--2019</v>
       </c>
       <c r="G11" t="s">
-        <v>39</v>
+        <v>52</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>36</v>
+        <v>64</v>
       </c>
       <c r="B12" t="s">
-        <v>37</v>
+        <v>29</v>
       </c>
       <c r="C12" t="s">
-        <v>38</v>
+        <v>27</v>
       </c>
       <c r="D12">
-        <v>2014</v>
+        <v>2016</v>
       </c>
       <c r="E12">
-        <v>2019</v>
+        <v>2018</v>
       </c>
       <c r="F12" t="str">
-        <f>_xlfn.CONCAT(D12,"--",E12)</f>
-        <v>2014--2019</v>
+        <f t="shared" si="0"/>
+        <v>2016--2018</v>
       </c>
       <c r="G12" t="s">
-        <v>75</v>
+        <v>30</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="B13" t="s">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="C13" t="s">
-        <v>38</v>
+        <v>19</v>
       </c>
       <c r="D13">
-        <v>2014</v>
+        <v>2016</v>
       </c>
       <c r="E13">
-        <v>2019</v>
+        <v>2018</v>
       </c>
       <c r="F13" t="str">
-        <f>_xlfn.CONCAT(D13,"--",E13)</f>
-        <v>2014--2019</v>
+        <f t="shared" si="0"/>
+        <v>2016--2018</v>
       </c>
       <c r="G13" t="s">
-        <v>71</v>
+        <v>58</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
-        <v>40</v>
+        <v>65</v>
       </c>
       <c r="B14" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
       <c r="C14" t="s">
-        <v>38</v>
+        <v>19</v>
       </c>
       <c r="D14">
-        <v>2016</v>
+        <v>2011</v>
       </c>
       <c r="E14">
-        <v>2018</v>
+        <v>2011</v>
       </c>
       <c r="F14" t="str">
-        <f>_xlfn.CONCAT(D14,"--",E14)</f>
-        <v>2016--2018</v>
+        <f t="shared" si="0"/>
+        <v>2011--2011</v>
       </c>
       <c r="G14" t="s">
-        <v>42</v>
+        <v>71</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
-        <v>43</v>
+        <v>65</v>
       </c>
       <c r="B15" t="s">
-        <v>44</v>
+        <v>33</v>
       </c>
       <c r="C15" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="D15">
-        <v>2016</v>
+        <v>2011</v>
       </c>
       <c r="E15">
-        <v>2018</v>
+        <v>2011</v>
       </c>
       <c r="F15" t="str">
-        <f>_xlfn.CONCAT(D15,"--",E15)</f>
-        <v>2016--2018</v>
+        <f t="shared" si="0"/>
+        <v>2011--2011</v>
       </c>
       <c r="G15" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>43</v>
-      </c>
-      <c r="B16" t="s">
-        <v>44</v>
-      </c>
-      <c r="C16" t="s">
-        <v>22</v>
-      </c>
-      <c r="D16">
-        <v>2016</v>
-      </c>
-      <c r="E16">
-        <v>2018</v>
-      </c>
-      <c r="F16" t="str">
-        <f>_xlfn.CONCAT(D16,"--",E16)</f>
-        <v>2016--2018</v>
-      </c>
-      <c r="G16" t="s">
-        <v>79</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>45</v>
-      </c>
-      <c r="B17" t="s">
-        <v>46</v>
-      </c>
-      <c r="C17" t="s">
-        <v>22</v>
-      </c>
-      <c r="D17">
-        <v>2011</v>
-      </c>
-      <c r="E17">
-        <v>2011</v>
-      </c>
-      <c r="F17" t="str">
-        <f>_xlfn.CONCAT(D17,"--",E17)</f>
-        <v>2011--2011</v>
-      </c>
-      <c r="G17" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>45</v>
-      </c>
-      <c r="B18" t="s">
-        <v>46</v>
-      </c>
-      <c r="C18" t="s">
-        <v>22</v>
-      </c>
-      <c r="D18">
-        <v>2011</v>
-      </c>
-      <c r="E18">
-        <v>2011</v>
-      </c>
-      <c r="F18" t="str">
-        <f>_xlfn.CONCAT(D18,"--",E18)</f>
-        <v>2011--2011</v>
-      </c>
-      <c r="G18" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>45</v>
-      </c>
-      <c r="B19" t="s">
-        <v>46</v>
-      </c>
-      <c r="C19" t="s">
-        <v>22</v>
-      </c>
-      <c r="D19">
-        <v>2011</v>
-      </c>
-      <c r="E19">
-        <v>2011</v>
-      </c>
-      <c r="F19" t="str">
-        <f>_xlfn.CONCAT(D19,"--",E19)</f>
-        <v>2011--2011</v>
-      </c>
-      <c r="G19" t="s">
-        <v>77</v>
+        <v>57</v>
       </c>
     </row>
   </sheetData>
@@ -1225,92 +1109,167 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7F75B33B-21C6-D44F-A780-FE0F5972B759}">
-  <dimension ref="A1:B10"/>
+  <dimension ref="A1:D13"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B13" sqref="B13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2" s="2" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" s="2" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="C1" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="D1" s="2" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>75</v>
+      </c>
+      <c r="B2" t="s">
         <v>1</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="C2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>75</v>
+      </c>
+      <c r="B3" t="s">
+        <v>42</v>
+      </c>
+      <c r="C3">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>75</v>
+      </c>
+      <c r="B4" t="s">
+        <v>43</v>
+      </c>
+      <c r="C4">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>75</v>
+      </c>
+      <c r="B5" t="s">
+        <v>44</v>
+      </c>
+      <c r="C5">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>75</v>
+      </c>
+      <c r="B6" t="s">
+        <v>45</v>
+      </c>
+      <c r="C6">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>75</v>
+      </c>
+      <c r="B7" t="s">
+        <v>3</v>
+      </c>
+      <c r="C7">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>75</v>
+      </c>
+      <c r="B8" t="s">
+        <v>2</v>
+      </c>
+      <c r="C8">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>75</v>
+      </c>
+      <c r="B9" t="s">
+        <v>53</v>
+      </c>
+      <c r="C9">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>75</v>
+      </c>
+      <c r="B10" t="s">
+        <v>54</v>
+      </c>
+      <c r="C10">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>80</v>
+      </c>
+      <c r="B11" t="s">
+        <v>47</v>
+      </c>
+      <c r="C11">
+        <v>5</v>
+      </c>
+      <c r="D11" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>80</v>
+      </c>
+      <c r="B12" t="s">
+        <v>48</v>
+      </c>
+      <c r="C12">
+        <v>5</v>
+      </c>
+      <c r="D12" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>80</v>
+      </c>
+      <c r="B13" t="s">
+        <v>81</v>
+      </c>
+      <c r="C13">
         <v>3</v>
       </c>
-      <c r="B2">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>55</v>
-      </c>
-      <c r="B3">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>56</v>
-      </c>
-      <c r="B4">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>57</v>
-      </c>
-      <c r="B5">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>58</v>
-      </c>
-      <c r="B6">
-        <v>3.5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>5</v>
-      </c>
-      <c r="B7">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>4</v>
-      </c>
-      <c r="B8">
-        <v>1.5</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>72</v>
-      </c>
-      <c r="B9">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>73</v>
-      </c>
-      <c r="B10">
-        <v>2</v>
+      <c r="D13" t="s">
+        <v>78</v>
       </c>
     </row>
   </sheetData>
@@ -1319,53 +1278,6 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4F11614D-DA3D-433E-9F1A-54AF0890230D}">
-  <dimension ref="A1:B4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="1" spans="1:2" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A1" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>62</v>
-      </c>
-      <c r="B2" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>63</v>
-      </c>
-      <c r="B3" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>64</v>
-      </c>
-      <c r="B4" t="s">
-        <v>66</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9D85D00E-93F1-5A40-A255-93EE8D9FEFDC}">
   <dimension ref="A1:G4"/>
   <sheetViews>
@@ -1375,25 +1287,25 @@
   <sheetData>
     <row r="1" spans="1:7" s="2" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="E1" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>13</v>
-      </c>
       <c r="G1" s="2" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="15.6" x14ac:dyDescent="0.3">
@@ -1428,11 +1340,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B0C1DA58-DF2A-1948-9210-AF2DD0CDBCFC}">
   <dimension ref="A1:G3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G2" sqref="G2"/>
     </sheetView>
   </sheetViews>
@@ -1440,36 +1352,36 @@
   <sheetData>
     <row r="1" spans="1:7" s="2" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>0</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="D1" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="E1" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="F1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="E1" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>13</v>
-      </c>
       <c r="G1" s="2" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>47</v>
+        <v>34</v>
       </c>
       <c r="B2" t="s">
-        <v>51</v>
+        <v>38</v>
       </c>
       <c r="C2" t="s">
-        <v>49</v>
+        <v>36</v>
       </c>
       <c r="D2">
         <v>2013</v>
@@ -1482,18 +1394,18 @@
         <v>2013--2013</v>
       </c>
       <c r="G2" t="s">
-        <v>53</v>
+        <v>40</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>48</v>
+        <v>35</v>
       </c>
       <c r="B3" t="s">
-        <v>52</v>
+        <v>39</v>
       </c>
       <c r="C3" t="s">
-        <v>50</v>
+        <v>37</v>
       </c>
       <c r="D3">
         <v>2011</v>
@@ -1506,50 +1418,10 @@
         <v>2011--2011</v>
       </c>
       <c r="G3" t="s">
-        <v>54</v>
+        <v>41</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0EAB08D9-F926-4C17-A2A6-080E21F80BFB}">
-  <dimension ref="A1:G1"/>
-  <sheetViews>
-    <sheetView workbookViewId="0"/>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="1" max="1" width="38.81640625" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:7" s="2" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="A1" s="2" t="s">
-        <v>10</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>0</v>
-      </c>
-      <c r="C1" s="2" t="s">
-        <v>8</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>11</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>12</v>
-      </c>
-      <c r="F1" s="2" t="s">
-        <v>13</v>
-      </c>
-      <c r="G1" s="2" t="s">
-        <v>9</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
updated cv, added skills and summary
</commit_message>
<xml_diff>
--- a/shira_salingre_cv_data.xlsx
+++ b/shira_salingre_cv_data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shirasalin\Documents\Work\my_cv\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{088588A0-A600-4213-B1C9-FEC690F8CE28}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41B0C2CA-09EF-43BA-A0C3-F5050C78D864}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{F213A91E-98B5-B244-B12A-A608C8962BCD}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="233" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="113">
   <si>
     <t>institution</t>
   </si>
@@ -305,27 +305,12 @@
     <t>R Statistical programming language</t>
   </si>
   <si>
-    <t>Spreadsheets (Michrosoft Excel, Google Sheets)</t>
-  </si>
-  <si>
-    <t>10 years</t>
-  </si>
-  <si>
-    <t>SQL (simple queries, SQL Server)</t>
-  </si>
-  <si>
     <t>Shiny</t>
   </si>
   <si>
     <t>Canva</t>
   </si>
   <si>
-    <t>Data</t>
-  </si>
-  <si>
-    <t>Design</t>
-  </si>
-  <si>
     <t>Adobe Photoshop</t>
   </si>
   <si>
@@ -350,9 +335,6 @@
     <t>Notion</t>
   </si>
   <si>
-    <t>Web</t>
-  </si>
-  <si>
     <t>Trello</t>
   </si>
   <si>
@@ -384,6 +366,18 @@
   </si>
   <si>
     <t>Area</t>
+  </si>
+  <si>
+    <t>Coding Languages</t>
+  </si>
+  <si>
+    <t>Software</t>
+  </si>
+  <si>
+    <t>SQL</t>
+  </si>
+  <si>
+    <t>Google Sheets</t>
   </si>
 </sst>
 </file>
@@ -1351,10 +1345,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7F75B33B-21C6-D44F-A780-FE0F5972B759}">
-  <dimension ref="A1:D35"/>
+  <dimension ref="A1:D33"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D16" sqref="D16"/>
+      <selection activeCell="B27" sqref="B27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1364,7 +1358,7 @@
         <v>43</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>114</v>
+        <v>108</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>44</v>
@@ -1378,7 +1372,7 @@
         <v>45</v>
       </c>
       <c r="B2" t="s">
-        <v>93</v>
+        <v>109</v>
       </c>
       <c r="C2" t="s">
         <v>87</v>
@@ -1392,7 +1386,7 @@
         <v>45</v>
       </c>
       <c r="B3" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="C3" t="s">
         <v>32</v>
@@ -1406,7 +1400,7 @@
         <v>45</v>
       </c>
       <c r="B4" t="s">
-        <v>93</v>
+        <v>94</v>
       </c>
       <c r="C4" t="s">
         <v>33</v>
@@ -1420,7 +1414,7 @@
         <v>45</v>
       </c>
       <c r="B5" t="s">
-        <v>93</v>
+        <v>110</v>
       </c>
       <c r="C5" t="s">
         <v>34</v>
@@ -1434,7 +1428,7 @@
         <v>45</v>
       </c>
       <c r="B6" t="s">
-        <v>93</v>
+        <v>110</v>
       </c>
       <c r="C6" t="s">
         <v>35</v>
@@ -1448,10 +1442,10 @@
         <v>45</v>
       </c>
       <c r="B7" t="s">
-        <v>93</v>
+        <v>109</v>
       </c>
       <c r="C7" t="s">
-        <v>90</v>
+        <v>111</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -1459,7 +1453,7 @@
         <v>45</v>
       </c>
       <c r="B8" t="s">
-        <v>93</v>
+        <v>109</v>
       </c>
       <c r="C8" t="s">
         <v>1</v>
@@ -1470,7 +1464,7 @@
         <v>45</v>
       </c>
       <c r="B9" t="s">
-        <v>93</v>
+        <v>109</v>
       </c>
       <c r="C9" t="s">
         <v>38</v>
@@ -1481,7 +1475,7 @@
         <v>45</v>
       </c>
       <c r="B10" t="s">
-        <v>93</v>
+        <v>109</v>
       </c>
       <c r="C10" t="s">
         <v>39</v>
@@ -1492,7 +1486,7 @@
         <v>45</v>
       </c>
       <c r="B11" t="s">
-        <v>93</v>
+        <v>110</v>
       </c>
       <c r="C11" t="s">
         <v>51</v>
@@ -1502,9 +1496,6 @@
       <c r="A12" t="s">
         <v>49</v>
       </c>
-      <c r="B12" t="s">
-        <v>49</v>
-      </c>
       <c r="C12" t="s">
         <v>36</v>
       </c>
@@ -1516,9 +1507,6 @@
       <c r="A13" t="s">
         <v>49</v>
       </c>
-      <c r="B13" t="s">
-        <v>49</v>
-      </c>
       <c r="C13" t="s">
         <v>37</v>
       </c>
@@ -1530,9 +1518,6 @@
       <c r="A14" t="s">
         <v>49</v>
       </c>
-      <c r="B14" t="s">
-        <v>49</v>
-      </c>
       <c r="C14" t="s">
         <v>50</v>
       </c>
@@ -1545,13 +1530,10 @@
         <v>45</v>
       </c>
       <c r="B15" t="s">
-        <v>93</v>
+        <v>110</v>
       </c>
       <c r="C15" t="s">
-        <v>88</v>
-      </c>
-      <c r="D15" t="s">
-        <v>89</v>
+        <v>112</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
@@ -1559,10 +1541,10 @@
         <v>45</v>
       </c>
       <c r="B16" t="s">
-        <v>93</v>
+        <v>109</v>
       </c>
       <c r="C16" t="s">
-        <v>91</v>
+        <v>88</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
@@ -1570,10 +1552,10 @@
         <v>45</v>
       </c>
       <c r="B17" t="s">
-        <v>94</v>
+        <v>110</v>
       </c>
       <c r="C17" t="s">
-        <v>92</v>
+        <v>89</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
@@ -1581,10 +1563,10 @@
         <v>45</v>
       </c>
       <c r="B18" t="s">
-        <v>94</v>
+        <v>110</v>
       </c>
       <c r="C18" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
@@ -1592,10 +1574,10 @@
         <v>45</v>
       </c>
       <c r="B19" t="s">
-        <v>94</v>
+        <v>110</v>
       </c>
       <c r="C19" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
@@ -1603,10 +1585,10 @@
         <v>45</v>
       </c>
       <c r="B20" t="s">
-        <v>94</v>
+        <v>110</v>
       </c>
       <c r="C20" t="s">
-        <v>97</v>
+        <v>92</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
@@ -1614,10 +1596,10 @@
         <v>45</v>
       </c>
       <c r="B21" t="s">
-        <v>94</v>
+        <v>110</v>
       </c>
       <c r="C21" t="s">
-        <v>98</v>
+        <v>93</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
@@ -1625,10 +1607,10 @@
         <v>45</v>
       </c>
       <c r="B22" t="s">
-        <v>99</v>
+        <v>110</v>
       </c>
       <c r="C22" t="s">
-        <v>100</v>
+        <v>95</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
@@ -1636,10 +1618,10 @@
         <v>45</v>
       </c>
       <c r="B23" t="s">
-        <v>99</v>
+        <v>110</v>
       </c>
       <c r="C23" t="s">
-        <v>101</v>
+        <v>96</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
@@ -1647,10 +1629,10 @@
         <v>45</v>
       </c>
       <c r="B24" t="s">
-        <v>99</v>
+        <v>110</v>
       </c>
       <c r="C24" t="s">
-        <v>102</v>
+        <v>97</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
@@ -1658,111 +1640,74 @@
         <v>45</v>
       </c>
       <c r="B25" t="s">
-        <v>103</v>
+        <v>110</v>
       </c>
       <c r="C25" t="s">
-        <v>38</v>
+        <v>98</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>45</v>
-      </c>
-      <c r="B26" t="s">
+        <v>99</v>
+      </c>
+      <c r="C26" t="s">
         <v>103</v>
-      </c>
-      <c r="C26" t="s">
-        <v>39</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>45</v>
-      </c>
-      <c r="B27" t="s">
         <v>99</v>
       </c>
       <c r="C27" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="C28" t="s">
-        <v>109</v>
+        <v>104</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
+        <v>99</v>
+      </c>
+      <c r="C29" t="s">
         <v>105</v>
-      </c>
-      <c r="B29" t="s">
-        <v>93</v>
-      </c>
-      <c r="C29" t="s">
-        <v>112</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>105</v>
-      </c>
-      <c r="B30" t="s">
-        <v>93</v>
+        <v>99</v>
       </c>
       <c r="C30" t="s">
-        <v>110</v>
+        <v>100</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>105</v>
-      </c>
-      <c r="B31" t="s">
-        <v>93</v>
+        <v>99</v>
       </c>
       <c r="C31" t="s">
-        <v>111</v>
+        <v>101</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>105</v>
-      </c>
-      <c r="B32" t="s">
-        <v>93</v>
+        <v>99</v>
       </c>
       <c r="C32" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>105</v>
+        <v>99</v>
       </c>
       <c r="C33" t="s">
         <v>107</v>
-      </c>
-    </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A34" t="s">
-        <v>105</v>
-      </c>
-      <c r="C34" t="s">
-        <v>108</v>
-      </c>
-    </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
-        <v>105</v>
-      </c>
-      <c r="B35" t="s">
-        <v>93</v>
-      </c>
-      <c r="C35" t="s">
-        <v>113</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated some details on CV
</commit_message>
<xml_diff>
--- a/shira_salingre_cv_data.xlsx
+++ b/shira_salingre_cv_data.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26227"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shirasalin\Documents\Work\my_cv\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B1AB9F8-9EFF-4B83-ADF4-BBDD81E9E04D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53D92C5B-D3FC-4875-8BCB-31DFDB8005C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{F213A91E-98B5-B244-B12A-A608C8962BCD}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="116">
   <si>
     <t>institution</t>
   </si>
@@ -296,9 +296,6 @@
     <t>Guided a multitude of nature-conservation oriented tours, field trips and lectures.</t>
   </si>
   <si>
-    <t>R Statistical programming language</t>
-  </si>
-  <si>
     <t>Shiny</t>
   </si>
   <si>
@@ -371,13 +368,25 @@
     <t>SQL</t>
   </si>
   <si>
-    <t>Google Sheets</t>
-  </si>
-  <si>
     <t>Collaborated with team members and conducted statistical, spatial and ecological data analysis on the organisation’s flagship project.</t>
   </si>
   <si>
     <t>Wrote detailed technical documentation for the organisations database.</t>
+  </si>
+  <si>
+    <t>Remote</t>
+  </si>
+  <si>
+    <t>Tel Aviv, Israel/Hybrid</t>
+  </si>
+  <si>
+    <t>Israel/Remote</t>
+  </si>
+  <si>
+    <t>Google Workspace</t>
+  </si>
+  <si>
+    <t>R Programming Language</t>
   </si>
 </sst>
 </file>
@@ -817,7 +826,7 @@
   <dimension ref="A1:G22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G11" sqref="G11"/>
+      <selection activeCell="C18" sqref="C18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -855,6 +864,9 @@
       <c r="B2" t="s">
         <v>53</v>
       </c>
+      <c r="C2" t="s">
+        <v>111</v>
+      </c>
       <c r="D2">
         <v>2015</v>
       </c>
@@ -876,6 +888,9 @@
       <c r="B3" t="s">
         <v>53</v>
       </c>
+      <c r="C3" t="s">
+        <v>111</v>
+      </c>
       <c r="D3">
         <v>2015</v>
       </c>
@@ -897,6 +912,9 @@
       <c r="B4" t="s">
         <v>53</v>
       </c>
+      <c r="C4" t="s">
+        <v>111</v>
+      </c>
       <c r="D4">
         <v>2015</v>
       </c>
@@ -918,6 +936,9 @@
       <c r="B5" t="s">
         <v>53</v>
       </c>
+      <c r="C5" t="s">
+        <v>111</v>
+      </c>
       <c r="D5">
         <v>2015</v>
       </c>
@@ -939,6 +960,9 @@
       <c r="B6" t="s">
         <v>53</v>
       </c>
+      <c r="C6" t="s">
+        <v>111</v>
+      </c>
       <c r="D6">
         <v>2015</v>
       </c>
@@ -961,7 +985,7 @@
         <v>18</v>
       </c>
       <c r="C7" t="s">
-        <v>13</v>
+        <v>112</v>
       </c>
       <c r="D7">
         <v>2020</v>
@@ -985,7 +1009,7 @@
         <v>18</v>
       </c>
       <c r="C8" t="s">
-        <v>13</v>
+        <v>112</v>
       </c>
       <c r="D8">
         <v>2020</v>
@@ -998,7 +1022,7 @@
         <v>2020--2022</v>
       </c>
       <c r="G8" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
@@ -1009,7 +1033,7 @@
         <v>18</v>
       </c>
       <c r="C9" t="s">
-        <v>13</v>
+        <v>112</v>
       </c>
       <c r="D9">
         <v>2020</v>
@@ -1033,7 +1057,7 @@
         <v>18</v>
       </c>
       <c r="C10" t="s">
-        <v>13</v>
+        <v>112</v>
       </c>
       <c r="D10">
         <v>2020</v>
@@ -1046,7 +1070,7 @@
         <v>2020--2022</v>
       </c>
       <c r="G10" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
@@ -1129,7 +1153,7 @@
         <v>20</v>
       </c>
       <c r="C14" t="s">
-        <v>21</v>
+        <v>113</v>
       </c>
       <c r="D14">
         <v>2014</v>
@@ -1153,7 +1177,7 @@
         <v>20</v>
       </c>
       <c r="C15" t="s">
-        <v>21</v>
+        <v>113</v>
       </c>
       <c r="D15">
         <v>2014</v>
@@ -1177,7 +1201,7 @@
         <v>20</v>
       </c>
       <c r="C16" t="s">
-        <v>21</v>
+        <v>113</v>
       </c>
       <c r="D16">
         <v>2014</v>
@@ -1297,7 +1321,7 @@
         <v>79</v>
       </c>
       <c r="C21" t="s">
-        <v>13</v>
+        <v>112</v>
       </c>
       <c r="D21">
         <v>2018</v>
@@ -1321,7 +1345,7 @@
         <v>79</v>
       </c>
       <c r="C22" t="s">
-        <v>13</v>
+        <v>112</v>
       </c>
       <c r="D22">
         <v>2018</v>
@@ -1348,7 +1372,7 @@
   <dimension ref="A1:D33"/>
   <sheetViews>
     <sheetView topLeftCell="A15" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="B27" sqref="B27"/>
+      <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1358,7 +1382,7 @@
         <v>43</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>44</v>
@@ -1372,10 +1396,10 @@
         <v>45</v>
       </c>
       <c r="B2" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C2" t="s">
-        <v>85</v>
+        <v>115</v>
       </c>
       <c r="D2" t="s">
         <v>71</v>
@@ -1386,7 +1410,7 @@
         <v>45</v>
       </c>
       <c r="B3" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C3" t="s">
         <v>32</v>
@@ -1400,7 +1424,7 @@
         <v>45</v>
       </c>
       <c r="B4" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="C4" t="s">
         <v>33</v>
@@ -1414,7 +1438,7 @@
         <v>45</v>
       </c>
       <c r="B5" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C5" t="s">
         <v>34</v>
@@ -1428,7 +1452,7 @@
         <v>45</v>
       </c>
       <c r="B6" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C6" t="s">
         <v>35</v>
@@ -1442,10 +1466,10 @@
         <v>45</v>
       </c>
       <c r="B7" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C7" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -1453,7 +1477,7 @@
         <v>45</v>
       </c>
       <c r="B8" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C8" t="s">
         <v>1</v>
@@ -1464,7 +1488,7 @@
         <v>45</v>
       </c>
       <c r="B9" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C9" t="s">
         <v>38</v>
@@ -1475,7 +1499,7 @@
         <v>45</v>
       </c>
       <c r="B10" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C10" t="s">
         <v>39</v>
@@ -1486,7 +1510,7 @@
         <v>45</v>
       </c>
       <c r="B11" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C11" t="s">
         <v>51</v>
@@ -1530,10 +1554,10 @@
         <v>45</v>
       </c>
       <c r="B15" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C15" t="s">
-        <v>110</v>
+        <v>114</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
@@ -1541,10 +1565,10 @@
         <v>45</v>
       </c>
       <c r="B16" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="C16" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
@@ -1552,10 +1576,10 @@
         <v>45</v>
       </c>
       <c r="B17" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C17" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
@@ -1563,10 +1587,10 @@
         <v>45</v>
       </c>
       <c r="B18" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C18" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
@@ -1574,10 +1598,10 @@
         <v>45</v>
       </c>
       <c r="B19" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C19" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
@@ -1585,10 +1609,10 @@
         <v>45</v>
       </c>
       <c r="B20" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C20" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
@@ -1596,10 +1620,10 @@
         <v>45</v>
       </c>
       <c r="B21" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C21" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
@@ -1607,10 +1631,10 @@
         <v>45</v>
       </c>
       <c r="B22" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C22" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
@@ -1618,10 +1642,10 @@
         <v>45</v>
       </c>
       <c r="B23" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C23" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
@@ -1629,10 +1653,10 @@
         <v>45</v>
       </c>
       <c r="B24" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C24" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
@@ -1640,74 +1664,74 @@
         <v>45</v>
       </c>
       <c r="B25" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="C25" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C26" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C27" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C28" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C29" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
+        <v>96</v>
+      </c>
+      <c r="C30" t="s">
         <v>97</v>
-      </c>
-      <c r="C30" t="s">
-        <v>98</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C31" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C32" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C33" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated main cv and added languages
</commit_message>
<xml_diff>
--- a/shira_salingre_cv_data.xlsx
+++ b/shira_salingre_cv_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shirasalin\Documents\Work\my_cv\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{53D92C5B-D3FC-4875-8BCB-31DFDB8005C9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{403BD747-0DBA-419C-8A0F-26DAD61DF0B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{F213A91E-98B5-B244-B12A-A608C8962BCD}"/>
+    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15840" xr2:uid="{F213A91E-98B5-B244-B12A-A608C8962BCD}"/>
   </bookViews>
   <sheets>
     <sheet name="education" sheetId="10" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="115">
   <si>
     <t>institution</t>
   </si>
@@ -206,24 +206,9 @@
     <t>Present</t>
   </si>
   <si>
-    <t>Lead a collaborative project, coordinated between 9 organisations, including NGOs, governmental organisations, authorities and municipalities, and defined a strategic vision statement.</t>
-  </si>
-  <si>
-    <t>Developed a training program and successfully managed a seasonal, volunteer-based information centre on the beach, which operates 6 months of the year.</t>
-  </si>
-  <si>
-    <t>Collaborated with another researcher to assist with Polcat observations spatial data analysis.</t>
-  </si>
-  <si>
-    <t>Produced a full summary report of underwater research activity along the city’s coastline, including data visualisations and maps.</t>
-  </si>
-  <si>
     <t>Project ecologist &amp; Data analyst</t>
   </si>
   <si>
-    <t>Cleaned and wrangled ecological data of ~7000 observations from 4 years of monitoring work, from multiple data sources.</t>
-  </si>
-  <si>
     <t>Curated a database from 3 data sources, including tabular, relational and geospatial data, and generated a detailed scientific report, including data summaries, data visualisations, maps and discussion.</t>
   </si>
   <si>
@@ -239,9 +224,6 @@
     <t>Established and managed a shark and rays citizen science observation database with over 1,000 observations.</t>
   </si>
   <si>
-    <t>Presented full database analysis in a European conference.</t>
-  </si>
-  <si>
     <t>Collected hundreds of samples to create a timeseries of environmental indicators.</t>
   </si>
   <si>
@@ -287,12 +269,6 @@
     <t>Organised a database of &gt;40K observations and made it accessible for exploration.</t>
   </si>
   <si>
-    <t>Created and gathered professional content for the general public, including 5 marine wildlife posters and blog posts.</t>
-  </si>
-  <si>
-    <t>Lead 4 groups of BSc students in intensive week-long Mediterranean Sea ecology courses.</t>
-  </si>
-  <si>
     <t>Guided a multitude of nature-conservation oriented tours, field trips and lectures.</t>
   </si>
   <si>
@@ -387,6 +363,27 @@
   </si>
   <si>
     <t>R Programming Language</t>
+  </si>
+  <si>
+    <t>Led collaborative projects, coordinating between multiple stakeholders, including organisation, authorities, and professionals.</t>
+  </si>
+  <si>
+    <t>Data analysis for research projects. Each project required data sourcing, cleaning, analysis and reporting.</t>
+  </si>
+  <si>
+    <t>Professional adviser and project coordinator for a multitude of nature conservation projects, including content creation for professionals, and the general public.</t>
+  </si>
+  <si>
+    <t>Cleaned and wrangled ecological data of thousands of observations, across several years of monitoring work, from multiple data sources.</t>
+  </si>
+  <si>
+    <t>In this job I use my data analysis knogwledge, alongside communication skills and my ability to work independently, to deliver timely, reliable and useful results.</t>
+  </si>
+  <si>
+    <t>Mentored groups of BSc students in intensive week-long Mediterranean Sea ecology courses.</t>
+  </si>
+  <si>
+    <t>Presented full database and analysis in a European conference.</t>
   </si>
 </sst>
 </file>
@@ -437,10 +434,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -757,7 +755,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9C4AE3D1-7C9F-C24D-A42B-F2C4925E72DD}">
   <dimension ref="A1:E3"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
@@ -823,10 +821,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C980247-8D3C-E442-A656-D4E45E07EA31}">
-  <dimension ref="A1:G22"/>
+  <dimension ref="A1:H21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H21" sqref="H21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -834,7 +832,7 @@
     <col min="1" max="1" width="38.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" s="1" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:8" s="1" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>6</v>
       </c>
@@ -857,7 +855,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>52</v>
       </c>
@@ -865,7 +863,7 @@
         <v>53</v>
       </c>
       <c r="C2" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="D2">
         <v>2015</v>
@@ -878,10 +876,10 @@
         <v>2015--Present</v>
       </c>
       <c r="G2" t="s">
-        <v>55</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>52</v>
       </c>
@@ -889,7 +887,7 @@
         <v>53</v>
       </c>
       <c r="C3" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="D3">
         <v>2015</v>
@@ -898,14 +896,14 @@
         <v>54</v>
       </c>
       <c r="F3" t="str">
-        <f t="shared" ref="F3:F19" si="0">CONCATENATE(D3,"--",E3)</f>
+        <f t="shared" ref="F3:F18" si="0">CONCATENATE(D3,"--",E3)</f>
         <v>2015--Present</v>
       </c>
-      <c r="G3" t="s">
-        <v>56</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G3" s="3" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>52</v>
       </c>
@@ -913,7 +911,7 @@
         <v>53</v>
       </c>
       <c r="C4" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="D4">
         <v>2015</v>
@@ -926,10 +924,10 @@
         <v>2015--Present</v>
       </c>
       <c r="G4" t="s">
-        <v>82</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>52</v>
       </c>
@@ -937,7 +935,7 @@
         <v>53</v>
       </c>
       <c r="C5" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="D5">
         <v>2015</v>
@@ -946,46 +944,46 @@
         <v>54</v>
       </c>
       <c r="F5" t="str">
-        <f t="shared" ref="F5:F6" si="2">CONCATENATE(D5,"--",E5)</f>
+        <f t="shared" ref="F5" si="2">CONCATENATE(D5,"--",E5)</f>
         <v>2015--Present</v>
       </c>
       <c r="G5" t="s">
-        <v>57</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="B6" t="s">
-        <v>53</v>
+        <v>18</v>
       </c>
       <c r="C6" t="s">
+        <v>104</v>
+      </c>
+      <c r="D6">
+        <v>2020</v>
+      </c>
+      <c r="E6">
+        <v>2022</v>
+      </c>
+      <c r="F6" t="str">
+        <f t="shared" si="0"/>
+        <v>2020--2022</v>
+      </c>
+      <c r="G6" t="s">
         <v>111</v>
       </c>
-      <c r="D6">
-        <v>2015</v>
-      </c>
-      <c r="E6" t="s">
-        <v>54</v>
-      </c>
-      <c r="F6" t="str">
-        <f t="shared" si="2"/>
-        <v>2015--Present</v>
-      </c>
-      <c r="G6" t="s">
-        <v>58</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="B7" t="s">
         <v>18</v>
       </c>
       <c r="C7" t="s">
-        <v>112</v>
+        <v>104</v>
       </c>
       <c r="D7">
         <v>2020</v>
@@ -998,18 +996,18 @@
         <v>2020--2022</v>
       </c>
       <c r="G7" t="s">
-        <v>60</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="B8" t="s">
         <v>18</v>
       </c>
       <c r="C8" t="s">
-        <v>112</v>
+        <v>104</v>
       </c>
       <c r="D8">
         <v>2020</v>
@@ -1022,18 +1020,18 @@
         <v>2020--2022</v>
       </c>
       <c r="G8" t="s">
-        <v>109</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
       <c r="B9" t="s">
         <v>18</v>
       </c>
       <c r="C9" t="s">
-        <v>112</v>
+        <v>104</v>
       </c>
       <c r="D9">
         <v>2020</v>
@@ -1042,64 +1040,64 @@
         <v>2022</v>
       </c>
       <c r="F9" t="str">
+        <f t="shared" ref="F9" si="3">CONCATENATE(D9,"--",E9)</f>
+        <v>2020--2022</v>
+      </c>
+      <c r="G9" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>40</v>
+      </c>
+      <c r="B10" t="s">
+        <v>16</v>
+      </c>
+      <c r="C10" t="s">
+        <v>17</v>
+      </c>
+      <c r="D10">
+        <v>2019</v>
+      </c>
+      <c r="E10" t="s">
+        <v>54</v>
+      </c>
+      <c r="F10" t="str">
         <f t="shared" si="0"/>
-        <v>2020--2022</v>
-      </c>
-      <c r="G9" t="s">
-        <v>61</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>59</v>
-      </c>
-      <c r="B10" t="s">
-        <v>18</v>
-      </c>
-      <c r="C10" t="s">
-        <v>112</v>
-      </c>
-      <c r="D10">
-        <v>2020</v>
-      </c>
-      <c r="E10">
-        <v>2022</v>
-      </c>
-      <c r="F10" t="str">
-        <f t="shared" ref="F10" si="3">CONCATENATE(D10,"--",E10)</f>
-        <v>2020--2022</v>
+        <v>2019--Present</v>
       </c>
       <c r="G10" t="s">
-        <v>110</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>40</v>
+        <v>57</v>
       </c>
       <c r="B11" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="C11" t="s">
-        <v>17</v>
+        <v>21</v>
       </c>
       <c r="D11">
+        <v>2007</v>
+      </c>
+      <c r="E11">
         <v>2019</v>
-      </c>
-      <c r="E11" t="s">
-        <v>54</v>
       </c>
       <c r="F11" t="str">
         <f t="shared" si="0"/>
-        <v>2019--Present</v>
-      </c>
-      <c r="G11" t="s">
-        <v>83</v>
-      </c>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+        <v>2007--2019</v>
+      </c>
+      <c r="G11" s="2" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>62</v>
+        <v>57</v>
       </c>
       <c r="B12" t="s">
         <v>19</v>
@@ -1114,38 +1112,38 @@
         <v>2019</v>
       </c>
       <c r="F12" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="F12" si="4">CONCATENATE(D12,"--",E12)</f>
         <v>2007--2019</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>84</v>
-      </c>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>62</v>
+        <v>42</v>
       </c>
       <c r="B13" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C13" t="s">
-        <v>21</v>
+        <v>105</v>
       </c>
       <c r="D13">
-        <v>2007</v>
+        <v>2014</v>
       </c>
       <c r="E13">
         <v>2019</v>
       </c>
       <c r="F13" t="str">
-        <f t="shared" ref="F13" si="4">CONCATENATE(D13,"--",E13)</f>
-        <v>2007--2019</v>
-      </c>
-      <c r="G13" s="2" t="s">
-        <v>63</v>
-      </c>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="0"/>
+        <v>2014--2019</v>
+      </c>
+      <c r="H13" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>42</v>
       </c>
@@ -1153,7 +1151,7 @@
         <v>20</v>
       </c>
       <c r="C14" t="s">
-        <v>113</v>
+        <v>105</v>
       </c>
       <c r="D14">
         <v>2014</v>
@@ -1165,11 +1163,11 @@
         <f t="shared" si="0"/>
         <v>2014--2019</v>
       </c>
-      <c r="G14" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H14" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>42</v>
       </c>
@@ -1177,7 +1175,7 @@
         <v>20</v>
       </c>
       <c r="C15" t="s">
-        <v>113</v>
+        <v>105</v>
       </c>
       <c r="D15">
         <v>2014</v>
@@ -1189,43 +1187,43 @@
         <f t="shared" si="0"/>
         <v>2014--2019</v>
       </c>
-      <c r="G15" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H15" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B16" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="C16" t="s">
-        <v>113</v>
+        <v>21</v>
       </c>
       <c r="D16">
-        <v>2014</v>
+        <v>2016</v>
       </c>
       <c r="E16">
-        <v>2019</v>
+        <v>2018</v>
       </c>
       <c r="F16" t="str">
         <f t="shared" si="0"/>
-        <v>2014--2019</v>
-      </c>
-      <c r="G16" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+        <v>2016--2018</v>
+      </c>
+      <c r="H16" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
-        <v>41</v>
+        <v>24</v>
       </c>
       <c r="B17" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="C17" t="s">
-        <v>21</v>
+        <v>17</v>
       </c>
       <c r="D17">
         <v>2016</v>
@@ -1237,37 +1235,37 @@
         <f t="shared" si="0"/>
         <v>2016--2018</v>
       </c>
-      <c r="G17" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H17" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>24</v>
+        <v>62</v>
       </c>
       <c r="B18" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="C18" t="s">
         <v>17</v>
       </c>
       <c r="D18">
-        <v>2016</v>
+        <v>2017</v>
       </c>
       <c r="E18">
-        <v>2018</v>
+        <v>2017</v>
       </c>
       <c r="F18" t="str">
         <f t="shared" si="0"/>
-        <v>2016--2018</v>
-      </c>
-      <c r="G18" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+        <v>2017--2017</v>
+      </c>
+      <c r="H18" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="B19" t="s">
         <v>26</v>
@@ -1282,46 +1280,46 @@
         <v>2017</v>
       </c>
       <c r="F19" t="str">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="F19:F20" si="5">CONCATENATE(D19,"--",E19)</f>
         <v>2017--2017</v>
       </c>
-      <c r="G19" t="s">
-        <v>69</v>
-      </c>
-    </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="H19" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="B20" t="s">
-        <v>26</v>
+        <v>73</v>
       </c>
       <c r="C20" t="s">
-        <v>17</v>
+        <v>104</v>
       </c>
       <c r="D20">
-        <v>2017</v>
+        <v>2018</v>
       </c>
       <c r="E20">
-        <v>2017</v>
+        <v>2020</v>
       </c>
       <c r="F20" t="str">
-        <f t="shared" ref="F20:F21" si="5">CONCATENATE(D20,"--",E20)</f>
-        <v>2017--2017</v>
-      </c>
-      <c r="G20" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
+        <f t="shared" si="5"/>
+        <v>2018--2020</v>
+      </c>
+      <c r="H20" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="B21" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="C21" t="s">
-        <v>112</v>
+        <v>104</v>
       </c>
       <c r="D21">
         <v>2018</v>
@@ -1330,35 +1328,11 @@
         <v>2020</v>
       </c>
       <c r="F21" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" ref="F21" si="6">CONCATENATE(D21,"--",E21)</f>
         <v>2018--2020</v>
       </c>
-      <c r="G21" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22" t="s">
-        <v>78</v>
-      </c>
-      <c r="B22" t="s">
-        <v>79</v>
-      </c>
-      <c r="C22" t="s">
-        <v>112</v>
-      </c>
-      <c r="D22">
-        <v>2018</v>
-      </c>
-      <c r="E22">
-        <v>2020</v>
-      </c>
-      <c r="F22" t="str">
-        <f t="shared" ref="F22" si="6">CONCATENATE(D22,"--",E22)</f>
-        <v>2018--2020</v>
-      </c>
-      <c r="G22" t="s">
-        <v>81</v>
+      <c r="H21" t="s">
+        <v>75</v>
       </c>
     </row>
   </sheetData>
@@ -1371,7 +1345,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7F75B33B-21C6-D44F-A780-FE0F5972B759}">
   <dimension ref="A1:D33"/>
   <sheetViews>
-    <sheetView topLeftCell="A15" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="C3" sqref="C3"/>
     </sheetView>
   </sheetViews>
@@ -1382,13 +1356,13 @@
         <v>43</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>105</v>
+        <v>97</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>44</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -1396,13 +1370,13 @@
         <v>45</v>
       </c>
       <c r="B2" t="s">
-        <v>106</v>
+        <v>98</v>
       </c>
       <c r="C2" t="s">
-        <v>115</v>
+        <v>107</v>
       </c>
       <c r="D2" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -1410,13 +1384,13 @@
         <v>45</v>
       </c>
       <c r="B3" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="C3" t="s">
         <v>32</v>
       </c>
       <c r="D3" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.25">
@@ -1424,13 +1398,13 @@
         <v>45</v>
       </c>
       <c r="B4" t="s">
-        <v>91</v>
+        <v>83</v>
       </c>
       <c r="C4" t="s">
         <v>33</v>
       </c>
       <c r="D4" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.25">
@@ -1438,13 +1412,13 @@
         <v>45</v>
       </c>
       <c r="B5" t="s">
-        <v>107</v>
+        <v>99</v>
       </c>
       <c r="C5" t="s">
         <v>34</v>
       </c>
       <c r="D5" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.25">
@@ -1452,13 +1426,13 @@
         <v>45</v>
       </c>
       <c r="B6" t="s">
-        <v>107</v>
+        <v>99</v>
       </c>
       <c r="C6" t="s">
         <v>35</v>
       </c>
       <c r="D6" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.25">
@@ -1466,10 +1440,10 @@
         <v>45</v>
       </c>
       <c r="B7" t="s">
-        <v>106</v>
+        <v>98</v>
       </c>
       <c r="C7" t="s">
-        <v>108</v>
+        <v>100</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.25">
@@ -1477,7 +1451,7 @@
         <v>45</v>
       </c>
       <c r="B8" t="s">
-        <v>106</v>
+        <v>98</v>
       </c>
       <c r="C8" t="s">
         <v>1</v>
@@ -1488,7 +1462,7 @@
         <v>45</v>
       </c>
       <c r="B9" t="s">
-        <v>106</v>
+        <v>98</v>
       </c>
       <c r="C9" t="s">
         <v>38</v>
@@ -1499,7 +1473,7 @@
         <v>45</v>
       </c>
       <c r="B10" t="s">
-        <v>106</v>
+        <v>98</v>
       </c>
       <c r="C10" t="s">
         <v>39</v>
@@ -1510,7 +1484,7 @@
         <v>45</v>
       </c>
       <c r="B11" t="s">
-        <v>107</v>
+        <v>99</v>
       </c>
       <c r="C11" t="s">
         <v>51</v>
@@ -1554,10 +1528,10 @@
         <v>45</v>
       </c>
       <c r="B15" t="s">
-        <v>107</v>
+        <v>99</v>
       </c>
       <c r="C15" t="s">
-        <v>114</v>
+        <v>106</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.25">
@@ -1565,10 +1539,10 @@
         <v>45</v>
       </c>
       <c r="B16" t="s">
-        <v>106</v>
+        <v>98</v>
       </c>
       <c r="C16" t="s">
-        <v>85</v>
+        <v>77</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.25">
@@ -1576,10 +1550,10 @@
         <v>45</v>
       </c>
       <c r="B17" t="s">
-        <v>107</v>
+        <v>99</v>
       </c>
       <c r="C17" t="s">
-        <v>86</v>
+        <v>78</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.25">
@@ -1587,10 +1561,10 @@
         <v>45</v>
       </c>
       <c r="B18" t="s">
-        <v>107</v>
+        <v>99</v>
       </c>
       <c r="C18" t="s">
-        <v>87</v>
+        <v>79</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.25">
@@ -1598,10 +1572,10 @@
         <v>45</v>
       </c>
       <c r="B19" t="s">
-        <v>107</v>
+        <v>99</v>
       </c>
       <c r="C19" t="s">
-        <v>88</v>
+        <v>80</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.25">
@@ -1609,10 +1583,10 @@
         <v>45</v>
       </c>
       <c r="B20" t="s">
-        <v>107</v>
+        <v>99</v>
       </c>
       <c r="C20" t="s">
-        <v>89</v>
+        <v>81</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.25">
@@ -1620,10 +1594,10 @@
         <v>45</v>
       </c>
       <c r="B21" t="s">
-        <v>107</v>
+        <v>99</v>
       </c>
       <c r="C21" t="s">
-        <v>90</v>
+        <v>82</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.25">
@@ -1631,10 +1605,10 @@
         <v>45</v>
       </c>
       <c r="B22" t="s">
-        <v>107</v>
+        <v>99</v>
       </c>
       <c r="C22" t="s">
-        <v>92</v>
+        <v>84</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.25">
@@ -1642,10 +1616,10 @@
         <v>45</v>
       </c>
       <c r="B23" t="s">
-        <v>107</v>
+        <v>99</v>
       </c>
       <c r="C23" t="s">
-        <v>93</v>
+        <v>85</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.25">
@@ -1653,10 +1627,10 @@
         <v>45</v>
       </c>
       <c r="B24" t="s">
-        <v>107</v>
+        <v>99</v>
       </c>
       <c r="C24" t="s">
-        <v>94</v>
+        <v>86</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.25">
@@ -1664,74 +1638,74 @@
         <v>45</v>
       </c>
       <c r="B25" t="s">
-        <v>107</v>
+        <v>99</v>
       </c>
       <c r="C25" t="s">
-        <v>95</v>
+        <v>87</v>
       </c>
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
-        <v>96</v>
+        <v>88</v>
       </c>
       <c r="C26" t="s">
-        <v>100</v>
+        <v>92</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A27" t="s">
-        <v>96</v>
+        <v>88</v>
       </c>
       <c r="C27" t="s">
-        <v>103</v>
+        <v>95</v>
       </c>
     </row>
     <row r="28" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
-        <v>96</v>
+        <v>88</v>
       </c>
       <c r="C28" t="s">
-        <v>101</v>
+        <v>93</v>
       </c>
     </row>
     <row r="29" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A29" t="s">
-        <v>96</v>
+        <v>88</v>
       </c>
       <c r="C29" t="s">
-        <v>102</v>
+        <v>94</v>
       </c>
     </row>
     <row r="30" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
-        <v>96</v>
+        <v>88</v>
       </c>
       <c r="C30" t="s">
-        <v>97</v>
+        <v>89</v>
       </c>
     </row>
     <row r="31" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A31" t="s">
-        <v>96</v>
+        <v>88</v>
       </c>
       <c r="C31" t="s">
-        <v>98</v>
+        <v>90</v>
       </c>
     </row>
     <row r="32" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
-        <v>96</v>
+        <v>88</v>
       </c>
       <c r="C32" t="s">
-        <v>99</v>
+        <v>91</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
+        <v>88</v>
+      </c>
+      <c r="C33" t="s">
         <v>96</v>
-      </c>
-      <c r="C33" t="s">
-        <v>104</v>
       </c>
     </row>
   </sheetData>
@@ -1796,7 +1770,7 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="B3" t="s">
         <v>31</v>
@@ -1817,10 +1791,10 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="B4" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
       <c r="C4" t="s">
         <v>21</v>

</xml_diff>

<commit_message>
corrected some missing information
</commit_message>
<xml_diff>
--- a/shira_salingre_cv_data.xlsx
+++ b/shira_salingre_cv_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shirasalin\Documents\Work\my_cv\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{403BD747-0DBA-419C-8A0F-26DAD61DF0B9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0288B1B0-CAD2-4ADE-9C7C-EA8443ACD9D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-16320" windowWidth="29040" windowHeight="15840" xr2:uid="{F213A91E-98B5-B244-B12A-A608C8962BCD}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{F213A91E-98B5-B244-B12A-A608C8962BCD}"/>
   </bookViews>
   <sheets>
     <sheet name="education" sheetId="10" r:id="rId1"/>
@@ -434,11 +434,10 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -755,7 +754,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9C4AE3D1-7C9F-C24D-A42B-F2C4925E72DD}">
   <dimension ref="A1:E3"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
@@ -821,10 +820,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C980247-8D3C-E442-A656-D4E45E07EA31}">
-  <dimension ref="A1:H21"/>
+  <dimension ref="A1:G21"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H21" sqref="H21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G13" sqref="G13:G21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -832,7 +831,7 @@
     <col min="1" max="1" width="38.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="1" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" s="1" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>6</v>
       </c>
@@ -855,7 +854,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>52</v>
       </c>
@@ -879,7 +878,7 @@
         <v>109</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>52</v>
       </c>
@@ -899,11 +898,11 @@
         <f t="shared" ref="F3:F18" si="0">CONCATENATE(D3,"--",E3)</f>
         <v>2015--Present</v>
       </c>
-      <c r="G3" s="3" t="s">
+      <c r="G3" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>52</v>
       </c>
@@ -927,7 +926,7 @@
         <v>108</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>52</v>
       </c>
@@ -951,7 +950,7 @@
         <v>112</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>55</v>
       </c>
@@ -975,7 +974,7 @@
         <v>111</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>55</v>
       </c>
@@ -999,7 +998,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>55</v>
       </c>
@@ -1023,7 +1022,7 @@
         <v>56</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>55</v>
       </c>
@@ -1047,7 +1046,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>40</v>
       </c>
@@ -1071,7 +1070,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>57</v>
       </c>
@@ -1095,7 +1094,7 @@
         <v>76</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>57</v>
       </c>
@@ -1119,7 +1118,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>42</v>
       </c>
@@ -1139,11 +1138,11 @@
         <f t="shared" si="0"/>
         <v>2014--2019</v>
       </c>
-      <c r="H13" t="s">
+      <c r="G13" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>42</v>
       </c>
@@ -1163,11 +1162,11 @@
         <f t="shared" si="0"/>
         <v>2014--2019</v>
       </c>
-      <c r="H14" t="s">
+      <c r="G14" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>42</v>
       </c>
@@ -1187,11 +1186,11 @@
         <f t="shared" si="0"/>
         <v>2014--2019</v>
       </c>
-      <c r="H15" t="s">
+      <c r="G15" t="s">
         <v>114</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>41</v>
       </c>
@@ -1211,11 +1210,11 @@
         <f t="shared" si="0"/>
         <v>2016--2018</v>
       </c>
-      <c r="H16" t="s">
+      <c r="G16" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" t="s">
         <v>24</v>
       </c>
@@ -1235,11 +1234,11 @@
         <f t="shared" si="0"/>
         <v>2016--2018</v>
       </c>
-      <c r="H17" t="s">
+      <c r="G17" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
         <v>62</v>
       </c>
@@ -1259,11 +1258,11 @@
         <f t="shared" si="0"/>
         <v>2017--2017</v>
       </c>
-      <c r="H18" t="s">
+      <c r="G18" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>62</v>
       </c>
@@ -1283,11 +1282,11 @@
         <f t="shared" ref="F19:F20" si="5">CONCATENATE(D19,"--",E19)</f>
         <v>2017--2017</v>
       </c>
-      <c r="H19" t="s">
+      <c r="G19" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>72</v>
       </c>
@@ -1307,11 +1306,11 @@
         <f t="shared" si="5"/>
         <v>2018--2020</v>
       </c>
-      <c r="H20" t="s">
+      <c r="G20" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>72</v>
       </c>
@@ -1331,7 +1330,7 @@
         <f t="shared" ref="F21" si="6">CONCATENATE(D21,"--",E21)</f>
         <v>2018--2020</v>
       </c>
-      <c r="H21" t="s">
+      <c r="G21" t="s">
         <v>75</v>
       </c>
     </row>

</xml_diff>

<commit_message>
additions for highlighted skills
</commit_message>
<xml_diff>
--- a/shira_salingre_cv_data.xlsx
+++ b/shira_salingre_cv_data.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\shirasalin\Documents\Work\my_cv\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6E6F6AD3-028C-4B93-928F-B2ADB848D8EA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{34314BE1-FAFB-463C-8C9E-6B828D9245DC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{F213A91E-98B5-B244-B12A-A608C8962BCD}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="2" xr2:uid="{F213A91E-98B5-B244-B12A-A608C8962BCD}"/>
   </bookViews>
   <sheets>
     <sheet name="education" sheetId="10" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="218" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="219" uniqueCount="116">
   <si>
     <t>institution</t>
   </si>
@@ -197,9 +197,6 @@
     <t>Tableau</t>
   </si>
   <si>
-    <t>Marine ecology consultant</t>
-  </si>
-  <si>
     <t>Self-employed</t>
   </si>
   <si>
@@ -347,9 +344,6 @@
     <t>Wrote detailed technical documentation for the organisations database.</t>
   </si>
   <si>
-    <t>Remote</t>
-  </si>
-  <si>
     <t>Tel Aviv, Israel/Hybrid</t>
   </si>
   <si>
@@ -384,6 +378,15 @@
   </si>
   <si>
     <t>Managed teams of 70-100 volunteers.</t>
+  </si>
+  <si>
+    <t>Scientific consultant</t>
+  </si>
+  <si>
+    <t>Remote/Israel/Barcelona</t>
+  </si>
+  <si>
+    <t>Highlight</t>
   </si>
 </sst>
 </file>
@@ -822,8 +825,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8C980247-8D3C-E442-A656-D4E45E07EA31}">
   <dimension ref="A1:G21"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G19" sqref="G19"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -856,109 +859,109 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>113</v>
+      </c>
+      <c r="B2" t="s">
         <v>52</v>
       </c>
-      <c r="B2" t="s">
-        <v>53</v>
-      </c>
       <c r="C2" t="s">
-        <v>102</v>
+        <v>114</v>
       </c>
       <c r="D2">
         <v>2015</v>
       </c>
       <c r="E2" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F2" t="str">
         <f>CONCATENATE(D2,"--",E2)</f>
         <v>2015--Present</v>
       </c>
       <c r="G2" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
+        <v>113</v>
+      </c>
+      <c r="B3" t="s">
         <v>52</v>
       </c>
-      <c r="B3" t="s">
-        <v>53</v>
-      </c>
       <c r="C3" t="s">
-        <v>102</v>
+        <v>114</v>
       </c>
       <c r="D3">
         <v>2015</v>
       </c>
       <c r="E3" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F3" t="str">
         <f t="shared" ref="F3:F18" si="0">CONCATENATE(D3,"--",E3)</f>
         <v>2015--Present</v>
       </c>
       <c r="G3" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>113</v>
+      </c>
+      <c r="B4" t="s">
         <v>52</v>
       </c>
-      <c r="B4" t="s">
-        <v>53</v>
-      </c>
       <c r="C4" t="s">
-        <v>102</v>
+        <v>114</v>
       </c>
       <c r="D4">
         <v>2015</v>
       </c>
       <c r="E4" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F4" t="str">
         <f t="shared" ref="F4" si="1">CONCATENATE(D4,"--",E4)</f>
         <v>2015--Present</v>
       </c>
       <c r="G4" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
+        <v>113</v>
+      </c>
+      <c r="B5" t="s">
         <v>52</v>
       </c>
-      <c r="B5" t="s">
-        <v>53</v>
-      </c>
       <c r="C5" t="s">
-        <v>102</v>
+        <v>114</v>
       </c>
       <c r="D5">
         <v>2015</v>
       </c>
       <c r="E5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F5" t="str">
         <f t="shared" ref="F5" si="2">CONCATENATE(D5,"--",E5)</f>
         <v>2015--Present</v>
       </c>
       <c r="G5" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B6" t="s">
         <v>18</v>
       </c>
       <c r="C6" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="D6">
         <v>2020</v>
@@ -971,18 +974,18 @@
         <v>2020--2022</v>
       </c>
       <c r="G6" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B7" t="s">
         <v>18</v>
       </c>
       <c r="C7" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="D7">
         <v>2020</v>
@@ -995,18 +998,18 @@
         <v>2020--2022</v>
       </c>
       <c r="G7" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B8" t="s">
         <v>18</v>
       </c>
       <c r="C8" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="D8">
         <v>2020</v>
@@ -1019,18 +1022,18 @@
         <v>2020--2022</v>
       </c>
       <c r="G8" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B9" t="s">
         <v>18</v>
       </c>
       <c r="C9" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="D9">
         <v>2020</v>
@@ -1043,7 +1046,7 @@
         <v>2020--2022</v>
       </c>
       <c r="G9" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
@@ -1060,19 +1063,19 @@
         <v>2019</v>
       </c>
       <c r="E10" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="F10" t="str">
         <f t="shared" si="0"/>
         <v>2019--Present</v>
       </c>
       <c r="G10" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B11" t="s">
         <v>19</v>
@@ -1091,12 +1094,12 @@
         <v>2007--2019</v>
       </c>
       <c r="G11" s="2" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B12" t="s">
         <v>19</v>
@@ -1115,7 +1118,7 @@
         <v>2007--2019</v>
       </c>
       <c r="G12" s="2" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
@@ -1126,7 +1129,7 @@
         <v>20</v>
       </c>
       <c r="C13" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="D13">
         <v>2014</v>
@@ -1139,7 +1142,7 @@
         <v>2014--2019</v>
       </c>
       <c r="G13" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
@@ -1150,7 +1153,7 @@
         <v>20</v>
       </c>
       <c r="C14" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="D14">
         <v>2014</v>
@@ -1163,7 +1166,7 @@
         <v>2014--2019</v>
       </c>
       <c r="G14" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
@@ -1174,7 +1177,7 @@
         <v>20</v>
       </c>
       <c r="C15" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="D15">
         <v>2014</v>
@@ -1187,7 +1190,7 @@
         <v>2014--2019</v>
       </c>
       <c r="G15" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
@@ -1235,12 +1238,12 @@
         <v>2016--2018</v>
       </c>
       <c r="G17" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B18" t="s">
         <v>26</v>
@@ -1259,12 +1262,12 @@
         <v>2017--2017</v>
       </c>
       <c r="G18" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B19" t="s">
         <v>26</v>
@@ -1283,18 +1286,18 @@
         <v>2017--2017</v>
       </c>
       <c r="G19" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
+        <v>70</v>
+      </c>
+      <c r="B20" t="s">
         <v>71</v>
       </c>
-      <c r="B20" t="s">
-        <v>72</v>
-      </c>
       <c r="C20" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="D20">
         <v>2018</v>
@@ -1307,18 +1310,18 @@
         <v>2018--2020</v>
       </c>
       <c r="G20" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
+        <v>70</v>
+      </c>
+      <c r="B21" t="s">
         <v>71</v>
       </c>
-      <c r="B21" t="s">
-        <v>72</v>
-      </c>
       <c r="C21" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="D21">
         <v>2018</v>
@@ -1331,7 +1334,7 @@
         <v>2018--2020</v>
       </c>
       <c r="G21" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
   </sheetData>
@@ -1342,154 +1345,187 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7F75B33B-21C6-D44F-A780-FE0F5972B759}">
-  <dimension ref="A1:D33"/>
+  <dimension ref="A1:E33"/>
   <sheetViews>
-    <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:4" s="1" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:5" s="1" customFormat="1" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>43</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="C1" s="1" t="s">
         <v>44</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>67</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+        <v>66</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>115</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>45</v>
       </c>
       <c r="B2" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C2" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="D2" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+        <v>63</v>
+      </c>
+      <c r="E2" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>45</v>
       </c>
       <c r="B3" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C3" t="s">
         <v>32</v>
       </c>
       <c r="D3" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+        <v>63</v>
+      </c>
+      <c r="E3" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>45</v>
       </c>
       <c r="B4" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C4" t="s">
         <v>33</v>
       </c>
       <c r="D4" t="s">
-        <v>64</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+        <v>63</v>
+      </c>
+      <c r="E4" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>45</v>
       </c>
       <c r="B5" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C5" t="s">
         <v>34</v>
       </c>
       <c r="D5" t="s">
-        <v>66</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+        <v>65</v>
+      </c>
+      <c r="E5" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
         <v>45</v>
       </c>
       <c r="B6" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C6" t="s">
         <v>35</v>
       </c>
       <c r="D6" t="s">
-        <v>65</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+        <v>64</v>
+      </c>
+      <c r="E6" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
         <v>45</v>
       </c>
       <c r="B7" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C7" t="s">
-        <v>99</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+        <v>98</v>
+      </c>
+      <c r="E7" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>45</v>
       </c>
       <c r="B8" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C8" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E8" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>45</v>
       </c>
       <c r="B9" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C9" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E9" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>45</v>
       </c>
       <c r="B10" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C10" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E10" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>45</v>
       </c>
       <c r="B11" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C11" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E11" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>49</v>
       </c>
@@ -1500,7 +1536,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
         <v>49</v>
       </c>
@@ -1511,7 +1547,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>49</v>
       </c>
@@ -1522,189 +1558,222 @@
         <v>48</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
         <v>45</v>
       </c>
       <c r="B15" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C15" t="s">
-        <v>105</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
+        <v>103</v>
+      </c>
+      <c r="E15" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" t="s">
         <v>45</v>
       </c>
       <c r="B16" t="s">
+        <v>96</v>
+      </c>
+      <c r="C16" t="s">
+        <v>75</v>
+      </c>
+      <c r="E16" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>45</v>
+      </c>
+      <c r="B17" t="s">
         <v>97</v>
       </c>
-      <c r="C16" t="s">
+      <c r="C17" t="s">
         <v>76</v>
       </c>
-    </row>
-    <row r="17" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>45</v>
-      </c>
-      <c r="B17" t="s">
-        <v>98</v>
-      </c>
-      <c r="C17" t="s">
+      <c r="E17" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>45</v>
+      </c>
+      <c r="B18" t="s">
+        <v>97</v>
+      </c>
+      <c r="C18" t="s">
         <v>77</v>
       </c>
-    </row>
-    <row r="18" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>45</v>
-      </c>
-      <c r="B18" t="s">
-        <v>98</v>
-      </c>
-      <c r="C18" t="s">
+      <c r="E18" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>45</v>
+      </c>
+      <c r="B19" t="s">
+        <v>97</v>
+      </c>
+      <c r="C19" t="s">
         <v>78</v>
       </c>
-    </row>
-    <row r="19" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>45</v>
-      </c>
-      <c r="B19" t="s">
-        <v>98</v>
-      </c>
-      <c r="C19" t="s">
+      <c r="E19" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
+        <v>45</v>
+      </c>
+      <c r="B20" t="s">
+        <v>97</v>
+      </c>
+      <c r="C20" t="s">
         <v>79</v>
       </c>
-    </row>
-    <row r="20" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>45</v>
-      </c>
-      <c r="B20" t="s">
-        <v>98</v>
-      </c>
-      <c r="C20" t="s">
+      <c r="E20" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A21" t="s">
+        <v>45</v>
+      </c>
+      <c r="B21" t="s">
+        <v>97</v>
+      </c>
+      <c r="C21" t="s">
         <v>80</v>
       </c>
-    </row>
-    <row r="21" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A21" t="s">
-        <v>45</v>
-      </c>
-      <c r="B21" t="s">
-        <v>98</v>
-      </c>
-      <c r="C21" t="s">
-        <v>81</v>
-      </c>
-    </row>
-    <row r="22" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="E21" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>45</v>
       </c>
       <c r="B22" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="C22" t="s">
+        <v>82</v>
+      </c>
+      <c r="E22" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A23" t="s">
+        <v>45</v>
+      </c>
+      <c r="B23" t="s">
+        <v>97</v>
+      </c>
+      <c r="C23" t="s">
         <v>83</v>
       </c>
-    </row>
-    <row r="23" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A23" t="s">
-        <v>45</v>
-      </c>
-      <c r="B23" t="s">
-        <v>98</v>
-      </c>
-      <c r="C23" t="s">
+      <c r="E23" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>45</v>
+      </c>
+      <c r="B24" t="s">
+        <v>97</v>
+      </c>
+      <c r="C24" t="s">
         <v>84</v>
       </c>
-    </row>
-    <row r="24" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
-        <v>45</v>
-      </c>
-      <c r="B24" t="s">
-        <v>98</v>
-      </c>
-      <c r="C24" t="s">
+      <c r="E24" t="b">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>45</v>
+      </c>
+      <c r="B25" t="s">
+        <v>97</v>
+      </c>
+      <c r="C25" t="s">
         <v>85</v>
       </c>
-    </row>
-    <row r="25" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A25" t="s">
-        <v>45</v>
-      </c>
-      <c r="B25" t="s">
-        <v>98</v>
-      </c>
-      <c r="C25" t="s">
+      <c r="E25" t="b">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
         <v>86</v>
       </c>
-    </row>
-    <row r="26" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
+      <c r="C26" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
+        <v>86</v>
+      </c>
+      <c r="C27" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A28" t="s">
+        <v>86</v>
+      </c>
+      <c r="C28" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>86</v>
+      </c>
+      <c r="C29" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
+        <v>86</v>
+      </c>
+      <c r="C30" t="s">
         <v>87</v>
       </c>
-      <c r="C26" t="s">
-        <v>91</v>
-      </c>
-    </row>
-    <row r="27" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
-        <v>87</v>
-      </c>
-      <c r="C27" t="s">
-        <v>94</v>
-      </c>
-    </row>
-    <row r="28" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
-        <v>87</v>
-      </c>
-      <c r="C28" t="s">
-        <v>92</v>
-      </c>
-    </row>
-    <row r="29" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
-        <v>87</v>
-      </c>
-      <c r="C29" t="s">
-        <v>93</v>
-      </c>
-    </row>
-    <row r="30" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
-        <v>87</v>
-      </c>
-      <c r="C30" t="s">
+    </row>
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>86</v>
+      </c>
+      <c r="C31" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="31" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
-        <v>87</v>
-      </c>
-      <c r="C31" t="s">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>86</v>
+      </c>
+      <c r="C32" t="s">
         <v>89</v>
-      </c>
-    </row>
-    <row r="32" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A32" t="s">
-        <v>87</v>
-      </c>
-      <c r="C32" t="s">
-        <v>90</v>
       </c>
     </row>
     <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="C33" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
   </sheetData>
@@ -1769,7 +1838,7 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B3" t="s">
         <v>31</v>
@@ -1790,10 +1859,10 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
+        <v>68</v>
+      </c>
+      <c r="B4" t="s">
         <v>69</v>
-      </c>
-      <c r="B4" t="s">
-        <v>70</v>
       </c>
       <c r="C4" t="s">
         <v>21</v>

</xml_diff>